<commit_message>
working thru small example
</commit_message>
<xml_diff>
--- a/Scratch.xlsx
+++ b/Scratch.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bojangles/Documents/CS/are_you_the_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D94E5489-0069-6B4D-88F3-077DD0FD8251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{546E5CA1-1374-D740-A736-950D89777563}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{C0B1479F-55C8-FE48-A058-0BF45B8A0942}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" activeTab="3" xr2:uid="{C0B1479F-55C8-FE48-A058-0BF45B8A0942}"/>
   </bookViews>
   <sheets>
     <sheet name="progress_season_1" sheetId="2" r:id="rId1"/>
     <sheet name="S1" sheetId="1" r:id="rId2"/>
+    <sheet name="N=4 Template" sheetId="3" r:id="rId3"/>
+    <sheet name="N=4 Example" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">progress_season_1!$A$1:$E$91</definedName>
@@ -67,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="69">
   <si>
     <t>guy</t>
   </si>
@@ -202,6 +204,102 @@
   <si>
     <t>After ceremony</t>
   </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Let's say Path 11 has all Perfect Matches.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * For the first ceremony, they choose Path 1 and find out 2 of the matches are correct.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; We know that Path 1 has a probability of zero for having all Perfect Matches.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; So we can drop any paths that don't contain at least one of the matches in Path 1. Namely, Paths 7, 10, 12, 14, 15, 16, 19, 20, 23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; This leaves 14 paths that could have all perfect matches.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; And there's a 3/14 probability for all Non-Path 1 matches.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; Now, there is a 5/14 probability for any of the couples from Path 1 based on the number of remaining paths. BUT WE KNOW THAT 2 OF THE 4 ARE PMs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; For Path 1 couples, is their new prob. 1/2 for any one and (1/2)(1/2) = 1/4 for two of them to both be PMs?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; Does the info about 2 of 4 Path 1 matches change the probabilities for Non-Path 1 matches?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> * Let's say at the 2nd Ceremony, they choose Path 6.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; This results in a blackout: 0 of the 4 are PMs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; The following paths are dropped: 2, 3, 4, 5, 6, 8, 18, 24 leaving 6 paths remaining.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; (A, E) overlapped from Path 1, but was not one of the 2 PMs from the 1st Ceremony, so now there's a 2/3 chance that (B, F), (C, G), or (D, H) is a PM.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; We know that 2 of the couples (B, F), (C, G), and (D, H) must be in the final path, so we can eliminate any that only have one of them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --&gt; This drops paths 9, 13, 22 leaving 3 paths.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; Each of the paths (11, 17, 21) and each of the couples are equally likely.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ==&gt; CEREMONY RESULTS DETERMINE THE MINIMUM AND MAXIMUM NUMBER OF THOSE COUPLES THAT NEED TO BE IN A GIVEN PATH FOR IT TO HAVE ALL PM's.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; If they chose Path 11, they would win.</t>
+  </si>
+  <si>
+    <t>Next:</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> -&gt; If they chose Path 17, it would have 1 PM, eliminating that path and leaving 11 and 21.  IS IT A 50-50 CHANCE FOR THESE LAST TWO PATHS?</t>
+  </si>
+  <si>
+    <t>1st Ceremony (2)</t>
+  </si>
+  <si>
+    <t>2nd Ceremony (0)</t>
+  </si>
+  <si>
+    <t>3rd Ceremony (1)</t>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +309,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -264,8 +362,81 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="4" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="5" tint="0.79998168889431442"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0" tint="-0.14999847407452621"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,8 +490,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -343,13 +526,133 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,6 +673,48 @@
     <xf numFmtId="164" fontId="0" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="5" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="2" builtinId="27"/>
@@ -2362,8 +2707,8 @@
   </sheetPr>
   <dimension ref="A1:S45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="J37" sqref="J37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3020,48 +3365,48 @@
         <v>0.2</v>
       </c>
       <c r="C18" s="14">
-        <f t="shared" ref="C18" si="8">(7/10)/8</f>
+        <f>7/10/8</f>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="D18" s="17">
-        <f>(8/10)/9</f>
-        <v>8.8888888888888892E-2</v>
+        <f>(8/10)/9-(1/9-1/10)/9</f>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E18" s="14">
-        <f t="shared" ref="E18:F19" si="9">(7/10)/8</f>
+        <f t="shared" ref="E18:F19" si="8">(7/10)/8</f>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="F18" s="14">
+        <f t="shared" si="8"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="G18" s="14">
+        <f>8/10/8</f>
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="14">
+        <f t="shared" ref="H18:K19" si="9">(7/10)/8</f>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="I18" s="14">
         <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="G18" s="14">
-        <f t="shared" ref="E18:G27" si="10">(8/10)/8</f>
-        <v>0.1</v>
-      </c>
-      <c r="H18" s="14">
-        <f t="shared" ref="H18:K19" si="11">(7/10)/8</f>
+      <c r="J18" s="14">
+        <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="I18" s="14">
-        <f t="shared" si="11"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="J18" s="14">
-        <f t="shared" si="11"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
       <c r="K18" s="14">
-        <f t="shared" si="11"/>
+        <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="L18" s="18">
         <f>SUM($B18:$K18)</f>
-        <v>1.0013888888888889</v>
+        <v>1.0001543209876544</v>
       </c>
       <c r="M18" s="9">
         <f>L18-1</f>
-        <v>1.388888888888884E-3</v>
+        <v>1.543209876544438E-4</v>
       </c>
       <c r="N18">
         <f>8/10</f>
@@ -3084,44 +3429,44 @@
         <v>0.2</v>
       </c>
       <c r="D19" s="17">
-        <f>(8/10)/9</f>
-        <v>8.8888888888888892E-2</v>
+        <f>(8/10)/9-(1/9-1/10)/9</f>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E19" s="14">
+        <f t="shared" si="8"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="F19" s="14">
+        <f t="shared" si="8"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="G19" s="14">
+        <f>8/10/8</f>
+        <v>0.1</v>
+      </c>
+      <c r="H19" s="14">
         <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="F19" s="14">
+      <c r="I19" s="14">
         <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="G19" s="14">
-        <f t="shared" si="10"/>
-        <v>0.1</v>
-      </c>
-      <c r="H19" s="14">
-        <f t="shared" si="11"/>
+      <c r="J19" s="14">
+        <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="I19" s="14">
-        <f t="shared" si="11"/>
+      <c r="K19" s="14">
+        <f t="shared" si="9"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="J19" s="14">
-        <f t="shared" si="11"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="K19" s="14">
-        <f t="shared" si="11"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
       <c r="L19" s="18">
-        <f t="shared" ref="L19:L27" si="12">SUM($B19:$K19)</f>
-        <v>1.0013888888888889</v>
+        <f t="shared" ref="L19:L27" si="10">SUM($B19:$K19)</f>
+        <v>1.0001543209876544</v>
       </c>
       <c r="M19" s="9">
-        <f t="shared" ref="M19:M27" si="13">L19-1</f>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" ref="M19:M27" si="11">L19-1</f>
+        <v>1.543209876544438E-4</v>
       </c>
       <c r="N19">
         <v>9</v>
@@ -3144,50 +3489,49 @@
         <v>17</v>
       </c>
       <c r="B20" s="14">
-        <f>(8/10)/8</f>
+        <f>8/10/8</f>
         <v>0.1</v>
       </c>
       <c r="C20" s="14">
-        <f>(8/10)/8</f>
+        <f>8/10/8</f>
         <v>0.1</v>
       </c>
       <c r="D20" s="19">
-        <f>2/10</f>
         <v>0.2</v>
       </c>
       <c r="E20" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="E20:F20" si="12">8/10/8</f>
         <v>0.1</v>
       </c>
       <c r="F20" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.1</v>
       </c>
       <c r="G20" s="16">
         <v>0</v>
       </c>
       <c r="H20" s="14">
-        <f t="shared" ref="H20:K20" si="14">(8/10)/8</f>
+        <f t="shared" ref="H20:K20" si="13">8/10/8</f>
         <v>0.1</v>
       </c>
       <c r="I20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
       <c r="J20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
       <c r="K20" s="14">
-        <f t="shared" si="14"/>
+        <f t="shared" si="13"/>
         <v>0.1</v>
       </c>
       <c r="L20" s="18">
-        <f t="shared" si="12"/>
+        <f t="shared" si="10"/>
         <v>0.99999999999999989</v>
       </c>
       <c r="M20" s="9">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="N20" s="5">
@@ -3195,11 +3539,11 @@
         <v>8.8888888888888892E-2</v>
       </c>
       <c r="O20" s="5">
-        <f t="shared" ref="O20:P20" si="15">$N$18/O19</f>
+        <f t="shared" ref="O20:P20" si="14">$N$18/O19</f>
         <v>0.1</v>
       </c>
       <c r="P20" s="5">
-        <f t="shared" si="15"/>
+        <f t="shared" si="14"/>
         <v>0.1142857142857143</v>
       </c>
       <c r="R20" s="5">
@@ -3216,52 +3560,52 @@
         <v>19</v>
       </c>
       <c r="B21" s="14">
-        <f t="shared" ref="B21:K27" si="16">(7/10)/8</f>
+        <f t="shared" ref="B21:B27" si="15">(7/10)/8</f>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C21" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="C21:C27" si="16">7/10/8</f>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="D21" s="17">
-        <f t="shared" ref="B21:K27" si="17">(8/10)/9</f>
-        <v>8.8888888888888892E-2</v>
+        <f t="shared" ref="B19:K27" si="17">(8/10)/9-(1/9-1/10)/9</f>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E21" s="13">
         <f>2/10</f>
         <v>0.2</v>
       </c>
       <c r="F21" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" ref="C21:K27" si="18">(7/10)/8</f>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G21" s="14">
+        <f t="shared" ref="G21:G22" si="19">8/10/8</f>
+        <v>0.1</v>
+      </c>
+      <c r="H21" s="14">
+        <f t="shared" si="18"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="I21" s="14">
+        <f t="shared" si="18"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="J21" s="14">
+        <f t="shared" si="18"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="K21" s="14">
+        <f t="shared" si="18"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="L21" s="18">
         <f t="shared" si="10"/>
-        <v>0.1</v>
-      </c>
-      <c r="H21" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="I21" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="J21" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="K21" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="L21" s="18">
-        <f t="shared" si="12"/>
-        <v>1.0013888888888889</v>
+        <v>1.0001543209876542</v>
       </c>
       <c r="M21" s="9">
-        <f t="shared" si="13"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.5432098765422175E-4</v>
       </c>
       <c r="N21" s="7"/>
       <c r="O21" s="5">
@@ -3282,52 +3626,52 @@
         <v>21</v>
       </c>
       <c r="B22" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C22" s="14">
         <f t="shared" si="16"/>
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="D22" s="17">
-        <f t="shared" si="17"/>
+      <c r="D22" s="14">
+        <f t="shared" ref="B22:E22" si="20">(8/10)/9</f>
         <v>8.8888888888888892E-2</v>
       </c>
       <c r="E22" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
+        <f t="shared" si="20"/>
+        <v>8.8888888888888892E-2</v>
       </c>
       <c r="F22" s="13">
         <f>2/10</f>
         <v>0.2</v>
       </c>
       <c r="G22" s="14">
+        <f t="shared" si="19"/>
+        <v>0.1</v>
+      </c>
+      <c r="H22" s="14">
+        <f>(8/10)/9</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="I22" s="14">
+        <f t="shared" ref="I22:K22" si="21">(8/10)/9</f>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="J22" s="14">
+        <f t="shared" si="21"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="K22" s="14">
+        <f t="shared" si="21"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="L22" s="18">
         <f t="shared" si="10"/>
-        <v>0.1</v>
-      </c>
-      <c r="H22" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="I22" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="J22" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="K22" s="14">
-        <f t="shared" si="16"/>
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="L22" s="18">
-        <f t="shared" si="12"/>
-        <v>1.0013888888888889</v>
+        <v>1.0083333333333333</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" si="13"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="11"/>
+        <v>8.3333333333333037E-3</v>
       </c>
       <c r="O22" s="6">
         <f>O21/O19</f>
@@ -3342,53 +3686,52 @@
       <c r="A23" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="17">
-        <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
-      </c>
-      <c r="C23" s="17">
-        <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+      <c r="B23" s="14">
+        <f t="shared" si="15"/>
+        <v>8.7499999999999994E-2</v>
+      </c>
+      <c r="C23" s="14">
+        <f t="shared" si="16"/>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="D23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="F23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="G23" s="19">
-        <f>2/10</f>
         <v>0.2</v>
       </c>
       <c r="H23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="I23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="J23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="K23" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="L23" s="18">
-        <f t="shared" si="12"/>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>0.98858024691358048</v>
       </c>
       <c r="M23" s="9">
-        <f t="shared" si="13"/>
-        <v>0</v>
+        <f t="shared" si="11"/>
+        <v>-1.1419753086419515E-2</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.2">
@@ -3396,7 +3739,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C24" s="14">
@@ -3405,18 +3748,18 @@
       </c>
       <c r="D24" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E24" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="F24" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G24" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="G24:G27" si="22">8/10/8</f>
         <v>0.1</v>
       </c>
       <c r="H24" s="13">
@@ -3424,24 +3767,24 @@
         <v>0.2</v>
       </c>
       <c r="I24" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="J24" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="K24" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="L24" s="18">
-        <f t="shared" si="12"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="10"/>
+        <v>1.0001543209876542</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" si="13"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.5432098765422175E-4</v>
       </c>
       <c r="N24" s="8">
         <f>(8/10)/9-(1/8-1/9)/8</f>
@@ -3453,7 +3796,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C25" s="14">
@@ -3462,22 +3805,22 @@
       </c>
       <c r="D25" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="F25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G25" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
       <c r="H25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="I25" s="13">
@@ -3485,20 +3828,20 @@
         <v>0.2</v>
       </c>
       <c r="J25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="K25" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="L25" s="18">
-        <f t="shared" si="12"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="10"/>
+        <v>1.0001543209876544</v>
       </c>
       <c r="M25" s="9">
-        <f t="shared" si="13"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.543209876544438E-4</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.2">
@@ -3506,7 +3849,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C26" s="14">
@@ -3515,26 +3858,26 @@
       </c>
       <c r="D26" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E26" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="F26" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G26" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
       <c r="H26" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="I26" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="J26" s="13">
@@ -3542,16 +3885,16 @@
         <v>0.2</v>
       </c>
       <c r="K26" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="L26" s="18">
-        <f t="shared" si="12"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="10"/>
+        <v>1.0001543209876542</v>
       </c>
       <c r="M26" s="9">
-        <f t="shared" si="13"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.5432098765422175E-4</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.2">
@@ -3559,7 +3902,7 @@
         <v>27</v>
       </c>
       <c r="B27" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="15"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="C27" s="14">
@@ -3568,30 +3911,30 @@
       </c>
       <c r="D27" s="17">
         <f t="shared" si="17"/>
-        <v>8.8888888888888892E-2</v>
+        <v>8.7654320987654327E-2</v>
       </c>
       <c r="E27" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="F27" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="G27" s="14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="22"/>
         <v>0.1</v>
       </c>
       <c r="H27" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="I27" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="J27" s="14">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>8.7499999999999994E-2</v>
       </c>
       <c r="K27" s="13">
@@ -3599,12 +3942,16 @@
         <v>0.2</v>
       </c>
       <c r="L27" s="18">
-        <f t="shared" si="12"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="10"/>
+        <v>1.0001543209876544</v>
       </c>
       <c r="M27" s="9">
-        <f t="shared" si="13"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="11"/>
+        <v>1.543209876544438E-4</v>
+      </c>
+      <c r="O27">
+        <f>(1/8-1/9)</f>
+        <v>1.3888888888888895E-2</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -3613,86 +3960,90 @@
       </c>
       <c r="B28" s="18">
         <f>SUM(B$18:B$27)</f>
-        <v>1.0013888888888889</v>
+        <v>1</v>
       </c>
       <c r="C28" s="18">
-        <f t="shared" ref="C28:K28" si="18">SUM(C$18:C$27)</f>
-        <v>1.0013888888888889</v>
+        <f t="shared" ref="C28:K28" si="23">SUM(C$18:C$27)</f>
+        <v>1</v>
       </c>
       <c r="D28" s="18">
-        <f t="shared" si="18"/>
-        <v>1</v>
+        <f t="shared" si="23"/>
+        <v>0.9901234567901237</v>
       </c>
       <c r="E28" s="18">
-        <f t="shared" si="18"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="23"/>
+        <v>1.0015432098765433</v>
       </c>
       <c r="F28" s="18">
-        <f t="shared" si="18"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="23"/>
+        <v>1.0001543209876544</v>
       </c>
       <c r="G28" s="18">
-        <f t="shared" si="18"/>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="H28" s="18">
-        <f t="shared" si="18"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="23"/>
+        <v>1.0015432098765433</v>
       </c>
       <c r="I28" s="18">
-        <f t="shared" si="18"/>
-        <v>1.0013888888888891</v>
+        <f t="shared" si="23"/>
+        <v>1.0015432098765433</v>
       </c>
       <c r="J28" s="18">
-        <f t="shared" si="18"/>
-        <v>1.0013888888888889</v>
+        <f t="shared" si="23"/>
+        <v>1.0015432098765433</v>
       </c>
       <c r="K28" s="18">
-        <f t="shared" si="18"/>
-        <v>1.0013888888888891</v>
+        <f t="shared" si="23"/>
+        <v>1.0015432098765433</v>
       </c>
       <c r="L28" s="14"/>
+      <c r="O28">
+        <f>(1/9)-(1/10)</f>
+        <v>1.1111111111111099E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B29" s="9">
         <f>B28-1</f>
-        <v>1.388888888888884E-3</v>
+        <v>0</v>
       </c>
       <c r="C29" s="9">
-        <f t="shared" ref="C29:K29" si="19">C28-1</f>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" ref="C29:K29" si="24">C28-1</f>
+        <v>0</v>
       </c>
       <c r="D29" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="24"/>
+        <v>-9.8765432098762984E-3</v>
+      </c>
+      <c r="E29" s="9">
+        <f t="shared" si="24"/>
+        <v>1.5432098765433278E-3</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="24"/>
+        <v>1.543209876544438E-4</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
-      <c r="E29" s="9">
-        <f t="shared" si="19"/>
-        <v>1.388888888888884E-3</v>
-      </c>
-      <c r="F29" s="9">
-        <f t="shared" si="19"/>
-        <v>1.388888888888884E-3</v>
-      </c>
-      <c r="G29" s="9">
-        <f t="shared" si="19"/>
-        <v>0</v>
-      </c>
       <c r="H29" s="9">
-        <f t="shared" si="19"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="24"/>
+        <v>1.5432098765433278E-3</v>
       </c>
       <c r="I29" s="9">
-        <f t="shared" si="19"/>
-        <v>1.388888888889106E-3</v>
+        <f t="shared" si="24"/>
+        <v>1.5432098765433278E-3</v>
       </c>
       <c r="J29" s="9">
-        <f t="shared" si="19"/>
-        <v>1.388888888888884E-3</v>
+        <f t="shared" si="24"/>
+        <v>1.5432098765433278E-3</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" si="19"/>
-        <v>1.388888888889106E-3</v>
+        <f t="shared" si="24"/>
+        <v>1.5432098765433278E-3</v>
       </c>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -3748,35 +4099,35 @@
         <v>0.17876543209876544</v>
       </c>
       <c r="D34" s="17">
-        <f t="shared" ref="D34:K34" si="20">D3*(1+8/10)</f>
+        <f t="shared" ref="D34:K34" si="25">D3*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="E34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="J34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="K34" s="14">
-        <f t="shared" si="20"/>
+        <f t="shared" si="25"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="L34" s="18">
@@ -3793,7 +4144,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="14">
-        <f t="shared" ref="B35:K35" si="21">B4*(1+8/10)</f>
+        <f t="shared" ref="B35:K35" si="26">B4*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C35" s="13">
@@ -3801,43 +4152,43 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="D35" s="17">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="J35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="K35" s="14">
-        <f t="shared" si="21"/>
+        <f t="shared" si="26"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="L35" s="18">
-        <f t="shared" ref="L35:L43" si="22">SUM($B35:$K35)</f>
+        <f t="shared" ref="L35:L43" si="27">SUM($B35:$K35)</f>
         <v>1.7407407407407409</v>
       </c>
       <c r="M35" s="9">
-        <f t="shared" ref="M35:M43" si="23">L35-1</f>
+        <f t="shared" ref="M35:M43" si="28">L35-1</f>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -3846,11 +4197,11 @@
         <v>17</v>
       </c>
       <c r="B36" s="14">
-        <f t="shared" ref="B36:K36" si="24">B5*(1+8/10)</f>
+        <f t="shared" ref="B36:K36" si="29">B5*(1+8/10)</f>
         <v>0.19999999999999998</v>
       </c>
       <c r="C36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="D36" s="13">
@@ -3858,39 +4209,39 @@
         <v>0.13333333333333333</v>
       </c>
       <c r="E36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="F36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="G36" s="16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="H36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="I36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="J36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="K36" s="14">
-        <f t="shared" si="24"/>
+        <f t="shared" si="29"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="L36" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.7333333333333332</v>
       </c>
       <c r="M36" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.73333333333333317</v>
       </c>
       <c r="O36">
@@ -3902,15 +4253,15 @@
         <v>19</v>
       </c>
       <c r="B37" s="14">
-        <f t="shared" ref="B37:K37" si="25">B6*(1+8/10)</f>
+        <f t="shared" ref="B37:K37" si="30">B6*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D37" s="17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E37" s="13">
@@ -3918,35 +4269,35 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="F37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="J37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="K37" s="14">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="L37" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="M37" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -3955,19 +4306,19 @@
         <v>21</v>
       </c>
       <c r="B38" s="14">
-        <f t="shared" ref="B38:K38" si="26">B7*(1+8/10)</f>
+        <f t="shared" ref="B38:K38" si="31">B7*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D38" s="17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F38" s="13">
@@ -3975,31 +4326,31 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="G38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="J38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="K38" s="14">
-        <f t="shared" si="26"/>
+        <f t="shared" si="31"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="L38" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="M38" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -4008,23 +4359,23 @@
         <v>22</v>
       </c>
       <c r="B39" s="17">
-        <f t="shared" ref="B39:K39" si="27">B8*(1+8/10)</f>
+        <f t="shared" ref="B39:K39" si="32">B8*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C39" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D39" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E39" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F39" s="17">
-        <f t="shared" si="27"/>
+        <f t="shared" si="32"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G39" s="13">
@@ -4032,27 +4383,27 @@
         <v>0.13333333333333333</v>
       </c>
       <c r="H39" s="17">
+        <f t="shared" si="32"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="I39" s="17">
+        <f t="shared" si="32"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="J39" s="17">
+        <f t="shared" si="32"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="K39" s="17">
+        <f t="shared" si="32"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="L39" s="18">
         <f t="shared" si="27"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="I39" s="17">
-        <f t="shared" si="27"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="J39" s="17">
-        <f t="shared" si="27"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="K39" s="17">
-        <f t="shared" si="27"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="L39" s="18">
-        <f t="shared" si="22"/>
         <v>1.7333333333333336</v>
       </c>
       <c r="M39" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.73333333333333361</v>
       </c>
     </row>
@@ -4061,27 +4412,27 @@
         <v>24</v>
       </c>
       <c r="B40" s="14">
-        <f t="shared" ref="B40:K40" si="28">B9*(1+8/10)</f>
+        <f t="shared" ref="B40:K40" si="33">B9*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C40" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D40" s="17">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E40" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F40" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G40" s="14">
-        <f t="shared" si="28"/>
+        <f t="shared" si="33"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H40" s="13">
@@ -4089,23 +4440,23 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="I40" s="14">
+        <f t="shared" si="33"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="J40" s="14">
+        <f t="shared" si="33"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="K40" s="14">
+        <f t="shared" si="33"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="L40" s="18">
+        <f t="shared" si="27"/>
+        <v>1.7407407407407409</v>
+      </c>
+      <c r="M40" s="9">
         <f t="shared" si="28"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="J40" s="14">
-        <f t="shared" si="28"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="K40" s="14">
-        <f t="shared" si="28"/>
-        <v>0.17777777777777778</v>
-      </c>
-      <c r="L40" s="18">
-        <f t="shared" si="22"/>
-        <v>1.7407407407407409</v>
-      </c>
-      <c r="M40" s="9">
-        <f t="shared" si="23"/>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -4114,31 +4465,31 @@
         <v>25</v>
       </c>
       <c r="B41" s="14">
-        <f t="shared" ref="B41:K41" si="29">B10*(1+8/10)</f>
+        <f t="shared" ref="B41:K41" si="34">B10*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D41" s="17">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I41" s="13">
@@ -4146,19 +4497,19 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="J41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="K41" s="14">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="L41" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="M41" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -4167,35 +4518,35 @@
         <v>26</v>
       </c>
       <c r="B42" s="14">
-        <f t="shared" ref="B42:K42" si="30">B11*(1+8/10)</f>
+        <f t="shared" ref="B42:K42" si="35">B11*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D42" s="17">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="J42" s="13">
@@ -4203,15 +4554,15 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="K42" s="14">
-        <f t="shared" si="30"/>
+        <f t="shared" si="35"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="L42" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="M42" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -4220,39 +4571,39 @@
         <v>27</v>
       </c>
       <c r="B43" s="14">
-        <f t="shared" ref="B43:K43" si="31">B12*(1+8/10)</f>
+        <f t="shared" ref="B43:J43" si="36">B12*(1+8/10)</f>
         <v>0.17777777777777778</v>
       </c>
       <c r="C43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="D43" s="17">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="E43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="F43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="G43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.19999999999999998</v>
       </c>
       <c r="H43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="I43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="J43" s="14">
-        <f t="shared" si="31"/>
+        <f t="shared" si="36"/>
         <v>0.17777777777777778</v>
       </c>
       <c r="K43" s="13">
@@ -4260,11 +4611,11 @@
         <v>0.11851851851851852</v>
       </c>
       <c r="L43" s="18">
-        <f t="shared" si="22"/>
+        <f t="shared" si="27"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="M43" s="9">
-        <f t="shared" si="23"/>
+        <f t="shared" si="28"/>
         <v>0.74074074074074092</v>
       </c>
     </row>
@@ -4277,39 +4628,39 @@
         <v>1.7409876543209879</v>
       </c>
       <c r="C44" s="18">
-        <f t="shared" ref="C44:K44" si="32">SUM(C$34:C$43)</f>
+        <f t="shared" ref="C44:K44" si="37">SUM(C$34:C$43)</f>
         <v>1.7417283950617286</v>
       </c>
       <c r="D44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7333333333333336</v>
       </c>
       <c r="E44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="F44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="G44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7333333333333332</v>
       </c>
       <c r="H44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="I44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="J44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="K44" s="18">
-        <f t="shared" si="32"/>
+        <f t="shared" si="37"/>
         <v>1.7407407407407409</v>
       </c>
       <c r="L44" s="14"/>
@@ -4320,68 +4671,2839 @@
         <v>0.7409876543209879</v>
       </c>
       <c r="C45" s="9">
-        <f t="shared" ref="C45" si="33">C44-1</f>
+        <f t="shared" ref="C45" si="38">C44-1</f>
         <v>0.74172839506172861</v>
       </c>
       <c r="D45" s="9">
-        <f t="shared" ref="D45" si="34">D44-1</f>
+        <f t="shared" ref="D45" si="39">D44-1</f>
         <v>0.73333333333333361</v>
       </c>
       <c r="E45" s="9">
-        <f t="shared" ref="E45" si="35">E44-1</f>
+        <f t="shared" ref="E45" si="40">E44-1</f>
         <v>0.74074074074074092</v>
       </c>
       <c r="F45" s="9">
-        <f t="shared" ref="F45" si="36">F44-1</f>
+        <f t="shared" ref="F45" si="41">F44-1</f>
         <v>0.74074074074074092</v>
       </c>
       <c r="G45" s="9">
-        <f t="shared" ref="G45" si="37">G44-1</f>
+        <f t="shared" ref="G45" si="42">G44-1</f>
         <v>0.73333333333333317</v>
       </c>
       <c r="H45" s="9">
-        <f t="shared" ref="H45" si="38">H44-1</f>
+        <f t="shared" ref="H45" si="43">H44-1</f>
         <v>0.74074074074074092</v>
       </c>
       <c r="I45" s="9">
-        <f t="shared" ref="I45" si="39">I44-1</f>
+        <f t="shared" ref="I45" si="44">I44-1</f>
         <v>0.74074074074074092</v>
       </c>
       <c r="J45" s="9">
-        <f t="shared" ref="J45" si="40">J44-1</f>
+        <f t="shared" ref="J45" si="45">J44-1</f>
         <v>0.74074074074074092</v>
       </c>
       <c r="K45" s="9">
-        <f t="shared" ref="K45" si="41">K44-1</f>
+        <f t="shared" ref="K45" si="46">K44-1</f>
         <v>0.74074074074074092</v>
       </c>
       <c r="L45" s="1"/>
       <c r="M45" s="1"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B28:K28">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B44:K44">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="L18:L27">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>$L18=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B28:K28">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
-      <formula>1</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="L34:L43">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula>$L34=1</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B44:K44">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="83" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{200C657B-113D-DE49-AA5E-814C7940A07F}">
+  <dimension ref="B3:X42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5" customWidth="1"/>
+    <col min="20" max="20" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B3" s="20">
+        <v>1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="20">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="20">
+        <f>H3+1</f>
+        <v>3</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="20">
+        <f>N3+1</f>
+        <v>4</v>
+      </c>
+      <c r="U3" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="H4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="N4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="T4" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" s="12"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="12"/>
+    </row>
+    <row r="5" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="H5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="J5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="N5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="23"/>
+    </row>
+    <row r="6" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="12"/>
+      <c r="H6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="12"/>
+      <c r="J6" s="12"/>
+      <c r="K6" s="12"/>
+      <c r="L6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="12"/>
+      <c r="P6" s="12"/>
+      <c r="Q6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="12"/>
+      <c r="T6" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="12"/>
+      <c r="V6" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="12"/>
+      <c r="X6" s="12"/>
+    </row>
+    <row r="7" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="23"/>
+      <c r="N7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="T7" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B10" s="20">
+        <f>T3+1</f>
+        <v>5</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="20">
+        <f>B10+1</f>
+        <v>6</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="20">
+        <f>H10+1</f>
+        <v>7</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="20">
+        <f>N10+1</f>
+        <v>8</v>
+      </c>
+      <c r="U10" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V10" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X10" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="12"/>
+      <c r="E11" s="12"/>
+      <c r="F11" s="12"/>
+      <c r="H11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="12"/>
+      <c r="K11" s="12"/>
+      <c r="L11" s="12"/>
+      <c r="N11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="12"/>
+      <c r="P11" s="12"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T11" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="12"/>
+      <c r="V11" s="12"/>
+      <c r="W11" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X11" s="12"/>
+    </row>
+    <row r="12" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="E12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="23"/>
+      <c r="H12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
+      <c r="K12" s="23"/>
+      <c r="L12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" s="23"/>
+      <c r="Q12" s="23"/>
+      <c r="R12" s="23"/>
+      <c r="T12" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="U12" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+    </row>
+    <row r="13" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="12"/>
+      <c r="D13" s="12"/>
+      <c r="E13" s="12"/>
+      <c r="F13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="12"/>
+      <c r="J13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="12"/>
+      <c r="L13" s="12"/>
+      <c r="N13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="12"/>
+      <c r="T13" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13" s="12"/>
+      <c r="V13" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" s="12"/>
+      <c r="X13" s="12"/>
+    </row>
+    <row r="14" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="23"/>
+      <c r="D14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="23"/>
+      <c r="F14" s="23"/>
+      <c r="H14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="J14" s="23"/>
+      <c r="K14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="23"/>
+      <c r="N14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" s="23"/>
+      <c r="P14" s="23"/>
+      <c r="Q14" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R14" s="23"/>
+      <c r="T14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B17" s="20">
+        <f>T10+1</f>
+        <v>9</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="20">
+        <f>B17+1</f>
+        <v>10</v>
+      </c>
+      <c r="I17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="20">
+        <f>H17+1</f>
+        <v>11</v>
+      </c>
+      <c r="O17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T17" s="20">
+        <f>N17+1</f>
+        <v>12</v>
+      </c>
+      <c r="U17" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W17" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X17" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="12"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="12"/>
+      <c r="N18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="T18" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+    </row>
+    <row r="19" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="H19" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="23"/>
+      <c r="K19" s="23"/>
+      <c r="L19" s="23"/>
+      <c r="N19" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="23"/>
+      <c r="Q19" s="23"/>
+      <c r="R19" s="23"/>
+      <c r="T19" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V19" s="23"/>
+      <c r="W19" s="23"/>
+      <c r="X19" s="23"/>
+    </row>
+    <row r="20" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="12"/>
+      <c r="H20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="12"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="12"/>
+      <c r="L20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="12"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="R20" s="12"/>
+      <c r="T20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="12"/>
+      <c r="V20" s="12"/>
+      <c r="W20" s="12"/>
+      <c r="X20" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="23"/>
+      <c r="F21" s="23"/>
+      <c r="H21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="23"/>
+      <c r="J21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="23"/>
+      <c r="L21" s="23"/>
+      <c r="N21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="23"/>
+      <c r="P21" s="23"/>
+      <c r="Q21" s="23"/>
+      <c r="R21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U21" s="23"/>
+      <c r="V21" s="23"/>
+      <c r="W21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="X21" s="23"/>
+    </row>
+    <row r="24" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B24" s="20">
+        <f>T17+1</f>
+        <v>13</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="20">
+        <f>B24+1</f>
+        <v>14</v>
+      </c>
+      <c r="I24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" s="20">
+        <f>H24+1</f>
+        <v>15</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R24" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" s="20">
+        <f>N24+1</f>
+        <v>16</v>
+      </c>
+      <c r="U24" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V24" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W24" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X24" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="H25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="12"/>
+      <c r="J25" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="12"/>
+      <c r="L25" s="12"/>
+      <c r="N25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T25" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U25" s="12"/>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X25" s="12"/>
+    </row>
+    <row r="26" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="23"/>
+      <c r="H26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="23"/>
+      <c r="J26" s="23"/>
+      <c r="K26" s="23"/>
+      <c r="L26" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="23"/>
+      <c r="P26" s="23"/>
+      <c r="Q26" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R26" s="23"/>
+      <c r="T26" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="U26" s="23"/>
+      <c r="V26" s="23"/>
+      <c r="W26" s="23"/>
+      <c r="X26" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B27" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="H27" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="12"/>
+      <c r="K27" s="12"/>
+      <c r="L27" s="12"/>
+      <c r="N27" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="P27" s="12"/>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="12"/>
+      <c r="T27" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U27" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="V27" s="12"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="12"/>
+    </row>
+    <row r="28" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B28" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="23"/>
+      <c r="F28" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="23"/>
+      <c r="J28" s="23"/>
+      <c r="K28" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="23"/>
+      <c r="N28" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O28" s="23"/>
+      <c r="P28" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q28" s="23"/>
+      <c r="R28" s="23"/>
+      <c r="T28" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U28" s="23"/>
+      <c r="V28" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+    </row>
+    <row r="31" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B31" s="20">
+        <f>T24+1</f>
+        <v>17</v>
+      </c>
+      <c r="C31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="20">
+        <f>B31+1</f>
+        <v>18</v>
+      </c>
+      <c r="I31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" s="20">
+        <f>H31+1</f>
+        <v>19</v>
+      </c>
+      <c r="O31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P31" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T31" s="20">
+        <f>N31+1</f>
+        <v>20</v>
+      </c>
+      <c r="U31" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V31" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W31" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X31" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="12"/>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="H32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" s="12"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="12"/>
+      <c r="L32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T32" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U32" s="12"/>
+      <c r="V32" s="12"/>
+      <c r="W32" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X32" s="12"/>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B33" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="23"/>
+      <c r="D33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="23"/>
+      <c r="F33" s="23"/>
+      <c r="H33" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33" s="23"/>
+      <c r="J33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="23"/>
+      <c r="L33" s="23"/>
+      <c r="N33" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23"/>
+      <c r="Q33" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R33" s="23"/>
+      <c r="T33" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="U33" s="23"/>
+      <c r="V33" s="23"/>
+      <c r="W33" s="23"/>
+      <c r="X33" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B34" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="12"/>
+      <c r="H34" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="12"/>
+      <c r="K34" s="12"/>
+      <c r="L34" s="12"/>
+      <c r="N34" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" s="12"/>
+      <c r="P34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="12"/>
+      <c r="T34" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="12"/>
+      <c r="V34" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W34" s="12"/>
+      <c r="X34" s="12"/>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="23"/>
+      <c r="F35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="23"/>
+      <c r="J35" s="23"/>
+      <c r="K35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="L35" s="23"/>
+      <c r="N35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="P35" s="23"/>
+      <c r="Q35" s="23"/>
+      <c r="R35" s="23"/>
+      <c r="T35" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U35" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V35" s="23"/>
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B38" s="20">
+        <f>T31+1</f>
+        <v>21</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="20">
+        <f>B38+1</f>
+        <v>22</v>
+      </c>
+      <c r="I38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="J38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="N38" s="20">
+        <f>H38+1</f>
+        <v>23</v>
+      </c>
+      <c r="O38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="P38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="R38" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="T38" s="20">
+        <f>N38+1</f>
+        <v>24</v>
+      </c>
+      <c r="U38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="V38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="W38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="X38" s="21" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B39" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39" s="12"/>
+      <c r="J39" s="12"/>
+      <c r="K39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" s="12"/>
+      <c r="N39" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39" s="12"/>
+      <c r="P39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="12"/>
+      <c r="T39" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="U39" s="12"/>
+      <c r="V39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="W39" s="12"/>
+      <c r="X39" s="12"/>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="H40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="23"/>
+      <c r="J40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" s="23"/>
+      <c r="L40" s="23"/>
+      <c r="N40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" s="23"/>
+      <c r="P40" s="23"/>
+      <c r="Q40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="R40" s="23"/>
+      <c r="T40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="U40" s="23"/>
+      <c r="V40" s="23"/>
+      <c r="W40" s="23"/>
+      <c r="X40" s="23" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B41" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="H41" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="12"/>
+      <c r="J41" s="12"/>
+      <c r="K41" s="12"/>
+      <c r="L41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="N41" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="O41" s="12"/>
+      <c r="P41" s="12"/>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="T41" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="U41" s="12"/>
+      <c r="V41" s="12"/>
+      <c r="W41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X41" s="12"/>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B42" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="H42" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="N42" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="P42" s="23"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="23"/>
+      <c r="T42" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="U42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="V42" s="23"/>
+      <c r="W42" s="23"/>
+      <c r="X42" s="23"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8AAFFBA6-168E-4641-A9DA-6AEE41B39D5A}">
+  <dimension ref="B2:AA42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.83203125" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" customWidth="1"/>
+    <col min="8" max="8" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5" customWidth="1"/>
+    <col min="14" max="14" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.5" customWidth="1"/>
+    <col min="20" max="20" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="2.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="2.5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B3" s="39">
+        <v>1</v>
+      </c>
+      <c r="C3" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="H3" s="48">
+        <f>B3+1</f>
+        <v>2</v>
+      </c>
+      <c r="I3" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="K3" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="L3" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="N3" s="48">
+        <f>H3+1</f>
+        <v>3</v>
+      </c>
+      <c r="O3" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="P3" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q3" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="R3" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" s="48">
+        <f>N3+1</f>
+        <v>4</v>
+      </c>
+      <c r="U3" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA3" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B4" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
+      <c r="F4" s="44"/>
+      <c r="H4" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="50"/>
+      <c r="K4" s="50"/>
+      <c r="L4" s="50"/>
+      <c r="N4" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="O4" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="P4" s="50"/>
+      <c r="Q4" s="50"/>
+      <c r="R4" s="50"/>
+      <c r="T4" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="U4" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="V4" s="50"/>
+      <c r="W4" s="50"/>
+      <c r="X4" s="50"/>
+      <c r="AA4" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B5" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="43"/>
+      <c r="D5" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" s="43"/>
+      <c r="F5" s="44"/>
+      <c r="H5" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="N5" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="O5" s="52"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="U5" s="52"/>
+      <c r="V5" s="52"/>
+      <c r="W5" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="X5" s="52"/>
+      <c r="AA5" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B6" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="44"/>
+      <c r="H6" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="50"/>
+      <c r="J6" s="50"/>
+      <c r="K6" s="50"/>
+      <c r="L6" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" s="50"/>
+      <c r="P6" s="50"/>
+      <c r="Q6" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="R6" s="50"/>
+      <c r="T6" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="U6" s="50"/>
+      <c r="V6" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="50"/>
+      <c r="X6" s="50"/>
+      <c r="AA6" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="7" spans="2:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="46"/>
+      <c r="D7" s="46"/>
+      <c r="E7" s="46"/>
+      <c r="F7" s="47" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="52"/>
+      <c r="J7" s="52"/>
+      <c r="K7" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="L7" s="52"/>
+      <c r="N7" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="O7" s="52"/>
+      <c r="P7" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" s="52"/>
+      <c r="R7" s="52"/>
+      <c r="T7" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="U7" s="52"/>
+      <c r="V7" s="52"/>
+      <c r="W7" s="52"/>
+      <c r="X7" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA7" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AA8" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA9" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B10" s="48">
+        <f>T3+1</f>
+        <v>5</v>
+      </c>
+      <c r="C10" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="39">
+        <f>B10+1</f>
+        <v>6</v>
+      </c>
+      <c r="I10" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="J10" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="K10" s="40" t="s">
+        <v>43</v>
+      </c>
+      <c r="L10" s="41" t="s">
+        <v>44</v>
+      </c>
+      <c r="N10" s="34">
+        <f>H10+1</f>
+        <v>7</v>
+      </c>
+      <c r="O10" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q10" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="T10" s="48">
+        <f>N10+1</f>
+        <v>8</v>
+      </c>
+      <c r="U10" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="V10" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="W10" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="X10" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA10" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B11" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="50"/>
+      <c r="E11" s="50"/>
+      <c r="F11" s="50"/>
+      <c r="H11" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="J11" s="43"/>
+      <c r="K11" s="43"/>
+      <c r="L11" s="44"/>
+      <c r="N11" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+      <c r="R11" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="T11" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="U11" s="50"/>
+      <c r="V11" s="50"/>
+      <c r="W11" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="X11" s="50"/>
+      <c r="AA11" s="33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B12" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="F12" s="52"/>
+      <c r="H12" s="42" t="s">
+        <v>38</v>
+      </c>
+      <c r="I12" s="43"/>
+      <c r="J12" s="43"/>
+      <c r="K12" s="43"/>
+      <c r="L12" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="N12" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O12" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+      <c r="R12" s="38"/>
+      <c r="T12" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="U12" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="V12" s="52"/>
+      <c r="W12" s="52"/>
+      <c r="X12" s="52"/>
+    </row>
+    <row r="13" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B13" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="50"/>
+      <c r="D13" s="50"/>
+      <c r="E13" s="50"/>
+      <c r="F13" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="H13" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="K13" s="43"/>
+      <c r="L13" s="44"/>
+      <c r="N13" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="O13" s="36"/>
+      <c r="P13" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" s="36"/>
+      <c r="R13" s="36"/>
+      <c r="T13" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="U13" s="50"/>
+      <c r="V13" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="W13" s="50"/>
+      <c r="X13" s="50"/>
+    </row>
+    <row r="14" spans="2:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="H14" s="45" t="s">
+        <v>40</v>
+      </c>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="L14" s="47"/>
+      <c r="N14" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O14" s="38"/>
+      <c r="P14" s="38"/>
+      <c r="Q14" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="R14" s="38"/>
+      <c r="T14" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="U14" s="52"/>
+      <c r="V14" s="52"/>
+      <c r="W14" s="52"/>
+      <c r="X14" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA14" s="33" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="15" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="AA15" s="33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="AA16" s="33" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B17" s="55">
+        <f>T10+1</f>
+        <v>9</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="F17" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="34">
+        <f>B17+1</f>
+        <v>10</v>
+      </c>
+      <c r="I17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="J17" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K17" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="L17" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="N17" s="24">
+        <f>H17+1</f>
+        <v>11</v>
+      </c>
+      <c r="O17" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="P17" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q17" s="25" t="s">
+        <v>43</v>
+      </c>
+      <c r="R17" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="T17" s="34">
+        <f>N17+1</f>
+        <v>12</v>
+      </c>
+      <c r="U17" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="V17" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="W17" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="X17" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA17" s="54" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B18" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="57"/>
+      <c r="D18" s="57"/>
+      <c r="E18" s="57"/>
+      <c r="F18" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="36"/>
+      <c r="J18" s="36"/>
+      <c r="K18" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="36"/>
+      <c r="N18" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="O18" s="28"/>
+      <c r="P18" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q18" s="28"/>
+      <c r="R18" s="29"/>
+      <c r="T18" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="U18" s="36"/>
+      <c r="V18" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="W18" s="36"/>
+      <c r="X18" s="36"/>
+      <c r="AA18" s="33" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B19" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="59"/>
+      <c r="E19" s="59"/>
+      <c r="F19" s="59"/>
+      <c r="H19" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="I19" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="38"/>
+      <c r="K19" s="38"/>
+      <c r="L19" s="38"/>
+      <c r="N19" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="O19" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="28"/>
+      <c r="Q19" s="28"/>
+      <c r="R19" s="29"/>
+      <c r="T19" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="U19" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="V19" s="38"/>
+      <c r="W19" s="38"/>
+      <c r="X19" s="38"/>
+      <c r="AA19" s="33" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B20" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="57"/>
+      <c r="H20" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
+      <c r="K20" s="36"/>
+      <c r="L20" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="N20" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="O20" s="28"/>
+      <c r="P20" s="28"/>
+      <c r="Q20" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="R20" s="29"/>
+      <c r="T20" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="U20" s="36"/>
+      <c r="V20" s="36"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA20" s="33" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:27" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="59"/>
+      <c r="D21" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="H21" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="K21" s="38"/>
+      <c r="L21" s="38"/>
+      <c r="N21" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="T21" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="U21" s="38"/>
+      <c r="V21" s="38"/>
+      <c r="W21" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="X21" s="38"/>
+    </row>
+    <row r="24" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B24" s="55">
+        <f>T17+1</f>
+        <v>13</v>
+      </c>
+      <c r="C24" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="F24" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="H24" s="34">
+        <f>B24+1</f>
+        <v>14</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="J24" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K24" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="L24" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="N24" s="34">
+        <f>H24+1</f>
+        <v>15</v>
+      </c>
+      <c r="O24" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="P24" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q24" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="R24" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="T24" s="34">
+        <f>N24+1</f>
+        <v>16</v>
+      </c>
+      <c r="U24" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="V24" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="W24" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="X24" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="AA24" s="53" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B25" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="C25" s="57"/>
+      <c r="D25" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="57"/>
+      <c r="F25" s="57"/>
+      <c r="H25" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="36"/>
+      <c r="J25" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="K25" s="36"/>
+      <c r="L25" s="36"/>
+      <c r="N25" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O25" s="36"/>
+      <c r="P25" s="36"/>
+      <c r="Q25" s="36"/>
+      <c r="R25" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="T25" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="U25" s="36"/>
+      <c r="V25" s="36"/>
+      <c r="W25" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="X25" s="36"/>
+    </row>
+    <row r="26" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B26" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="F26" s="59"/>
+      <c r="H26" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
+      <c r="L26" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="N26" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O26" s="38"/>
+      <c r="P26" s="38"/>
+      <c r="Q26" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="R26" s="38"/>
+      <c r="T26" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="U26" s="38"/>
+      <c r="V26" s="38"/>
+      <c r="W26" s="38"/>
+      <c r="X26" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B27" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" s="57"/>
+      <c r="E27" s="57"/>
+      <c r="F27" s="57"/>
+      <c r="H27" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="I27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="J27" s="36"/>
+      <c r="K27" s="36"/>
+      <c r="L27" s="36"/>
+      <c r="N27" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="O27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="P27" s="36"/>
+      <c r="Q27" s="36"/>
+      <c r="R27" s="36"/>
+      <c r="T27" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="U27" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="V27" s="36"/>
+      <c r="W27" s="36"/>
+      <c r="X27" s="36"/>
+      <c r="AA27" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B28" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="H28" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="38"/>
+      <c r="J28" s="38"/>
+      <c r="K28" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="L28" s="38"/>
+      <c r="N28" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O28" s="38"/>
+      <c r="P28" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q28" s="38"/>
+      <c r="R28" s="38"/>
+      <c r="T28" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="U28" s="38"/>
+      <c r="V28" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="W28" s="38"/>
+      <c r="X28" s="38"/>
+      <c r="AA28" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B31" s="60">
+        <f>T24+1</f>
+        <v>17</v>
+      </c>
+      <c r="C31" s="61" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" s="61" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="61" t="s">
+        <v>43</v>
+      </c>
+      <c r="F31" s="61" t="s">
+        <v>44</v>
+      </c>
+      <c r="H31" s="48">
+        <f>B31+1</f>
+        <v>18</v>
+      </c>
+      <c r="I31" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="J31" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="K31" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="L31" s="49" t="s">
+        <v>44</v>
+      </c>
+      <c r="N31" s="34">
+        <f>H31+1</f>
+        <v>19</v>
+      </c>
+      <c r="O31" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="P31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="R31" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="T31" s="34">
+        <f>N31+1</f>
+        <v>20</v>
+      </c>
+      <c r="U31" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="V31" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="W31" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="X31" s="35" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="32" spans="2:27" x14ac:dyDescent="0.2">
+      <c r="B32" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" s="60"/>
+      <c r="D32" s="60"/>
+      <c r="E32" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="F32" s="60"/>
+      <c r="H32" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="I32" s="50"/>
+      <c r="J32" s="50"/>
+      <c r="K32" s="50"/>
+      <c r="L32" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="N32" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O32" s="36"/>
+      <c r="P32" s="36"/>
+      <c r="Q32" s="36"/>
+      <c r="R32" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="T32" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="U32" s="36"/>
+      <c r="V32" s="36"/>
+      <c r="W32" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="X32" s="36"/>
+    </row>
+    <row r="33" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B33" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" s="60"/>
+      <c r="D33" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="E33" s="60"/>
+      <c r="F33" s="60"/>
+      <c r="H33" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="I33" s="52"/>
+      <c r="J33" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="K33" s="52"/>
+      <c r="L33" s="52"/>
+      <c r="N33" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="R33" s="38"/>
+      <c r="T33" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="U33" s="38"/>
+      <c r="V33" s="38"/>
+      <c r="W33" s="38"/>
+      <c r="X33" s="38" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="34" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B34" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="D34" s="60"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="60"/>
+      <c r="H34" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="I34" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="J34" s="50"/>
+      <c r="K34" s="50"/>
+      <c r="L34" s="50"/>
+      <c r="N34" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="O34" s="36"/>
+      <c r="P34" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q34" s="36"/>
+      <c r="R34" s="36"/>
+      <c r="T34" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="U34" s="36"/>
+      <c r="V34" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="W34" s="36"/>
+      <c r="X34" s="36"/>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B35" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="60"/>
+      <c r="D35" s="60"/>
+      <c r="E35" s="60"/>
+      <c r="F35" s="60" t="s">
+        <v>45</v>
+      </c>
+      <c r="H35" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="L35" s="52"/>
+      <c r="N35" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O35" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="P35" s="38"/>
+      <c r="Q35" s="38"/>
+      <c r="R35" s="38"/>
+      <c r="T35" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="U35" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="V35" s="38"/>
+      <c r="W35" s="38"/>
+      <c r="X35" s="38"/>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B38" s="20">
+        <f>T31+1</f>
+        <v>21</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="D38" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>44</v>
+      </c>
+      <c r="H38" s="55">
+        <f>B38+1</f>
+        <v>22</v>
+      </c>
+      <c r="I38" s="56" t="s">
+        <v>41</v>
+      </c>
+      <c r="J38" s="56" t="s">
+        <v>42</v>
+      </c>
+      <c r="K38" s="56" t="s">
+        <v>43</v>
+      </c>
+      <c r="L38" s="56" t="s">
+        <v>44</v>
+      </c>
+      <c r="N38" s="34">
+        <f>H38+1</f>
+        <v>23</v>
+      </c>
+      <c r="O38" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="P38" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q38" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="R38" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="T38" s="48">
+        <f>N38+1</f>
+        <v>24</v>
+      </c>
+      <c r="U38" s="49" t="s">
+        <v>41</v>
+      </c>
+      <c r="V38" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="W38" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="X38" s="49" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B39" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+      <c r="E39" s="12"/>
+      <c r="F39" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="H39" s="56" t="s">
+        <v>37</v>
+      </c>
+      <c r="I39" s="57"/>
+      <c r="J39" s="57"/>
+      <c r="K39" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" s="57"/>
+      <c r="N39" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="O39" s="36"/>
+      <c r="P39" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q39" s="36"/>
+      <c r="R39" s="36"/>
+      <c r="T39" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="U39" s="50"/>
+      <c r="V39" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="W39" s="50"/>
+      <c r="X39" s="50"/>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B40" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="23"/>
+      <c r="D40" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E40" s="23"/>
+      <c r="F40" s="23"/>
+      <c r="H40" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="59"/>
+      <c r="J40" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="N40" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="O40" s="38"/>
+      <c r="P40" s="38"/>
+      <c r="Q40" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="R40" s="38"/>
+      <c r="T40" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="U40" s="52"/>
+      <c r="V40" s="52"/>
+      <c r="W40" s="52"/>
+      <c r="X40" s="52" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B41" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="12"/>
+      <c r="H41" s="56" t="s">
+        <v>39</v>
+      </c>
+      <c r="I41" s="57"/>
+      <c r="J41" s="57"/>
+      <c r="K41" s="57"/>
+      <c r="L41" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="N41" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="O41" s="36"/>
+      <c r="P41" s="36"/>
+      <c r="Q41" s="36"/>
+      <c r="R41" s="36" t="s">
+        <v>45</v>
+      </c>
+      <c r="T41" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="U41" s="50"/>
+      <c r="V41" s="50"/>
+      <c r="W41" s="50" t="s">
+        <v>45</v>
+      </c>
+      <c r="X41" s="50"/>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.2">
+      <c r="B42" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="D42" s="23"/>
+      <c r="E42" s="23"/>
+      <c r="F42" s="23"/>
+      <c r="H42" s="58" t="s">
+        <v>40</v>
+      </c>
+      <c r="I42" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="N42" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="O42" s="38" t="s">
+        <v>45</v>
+      </c>
+      <c r="P42" s="38"/>
+      <c r="Q42" s="38"/>
+      <c r="R42" s="38"/>
+      <c r="T42" s="51" t="s">
+        <v>40</v>
+      </c>
+      <c r="U42" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="V42" s="52"/>
+      <c r="W42" s="52"/>
+      <c r="X42" s="52"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>